<commit_message>
added script to create linear programming scripts
</commit_message>
<xml_diff>
--- a/COMP321720212022CW2A/COMP3217CW2Input.xlsx
+++ b/COMP321720212022CW2A/COMP3217CW2Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiyan-adm\Desktop\Southampton\COMP3217\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/cb6g19_soton_ac_uk/Documents/Year 3/Semester 2/COMP3217/Labs/Lab2/COMP321720212022CW2A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D9FAC0-B77C-49D3-9C53-174903027F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{09D9FAC0-B77C-49D3-9C53-174903027F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE56B48B-7231-4B32-BFA4-0579C38D952A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE4D9E89-ED3E-9F4F-B454-34A6DA40E3CF}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{DE4D9E89-ED3E-9F4F-B454-34A6DA40E3CF}"/>
   </bookViews>
   <sheets>
     <sheet name="User &amp; Task ID" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NormalGuidelinePricing!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -297,10 +306,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,21 +625,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D33648-2EBE-814D-9D1C-C2A4EAB0BD48}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="14.796875" customWidth="1"/>
-    <col min="4" max="4" width="30.796875" customWidth="1"/>
-    <col min="5" max="5" width="17.19921875" customWidth="1"/>
-    <col min="9" max="9" width="13.8984375" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -646,7 +656,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -662,8 +672,9 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -679,8 +690,9 @@
       <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -696,8 +708,9 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -713,8 +726,9 @@
       <c r="E5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -730,8 +744,9 @@
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -747,8 +762,9 @@
       <c r="E7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -764,8 +780,9 @@
       <c r="E8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -781,8 +798,9 @@
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -798,8 +816,9 @@
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -815,8 +834,9 @@
       <c r="E11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -832,8 +852,9 @@
       <c r="E12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -849,8 +870,9 @@
       <c r="E13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -866,8 +888,9 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -883,8 +906,9 @@
       <c r="E15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -900,8 +924,9 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -917,8 +942,9 @@
       <c r="E17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -934,8 +960,9 @@
       <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -951,8 +978,9 @@
       <c r="E19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -968,8 +996,9 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -985,8 +1014,9 @@
       <c r="E21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1002,8 +1032,9 @@
       <c r="E22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1019,8 +1050,9 @@
       <c r="E23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1036,8 +1068,9 @@
       <c r="E24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1053,8 +1086,9 @@
       <c r="E25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1088,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1105,7 +1139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1122,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1139,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1156,7 +1190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1505,15 +1539,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75EF9C1-8F25-C149-B769-8319BA594532}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1521,196 +1555,268 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>4.2465223767728215</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>3.6400277961434484</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>3.4805026391870144</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>3.2454609947025612</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <v>3.1629159918690348</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>3.5976674954444445</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>3.9053559544181216</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <v>4.0783402462878993</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <v>5.3747974263961735</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>4.9446991235837698</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>5.4381000827159394</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <v>3.909231366353989</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <v>6.2006667261940969</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <v>4.4821418941480484</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <v>5.41080155790966</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
         <v>6.1491709685010445</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
         <v>5.883768700097348</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
         <v>6.3292632076075481</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <v>6.4695111523786952</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
         <v>5.5834976200853035</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
         <v>5.5589223785757591</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
         <v>5.2553547974771586</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <v>5.5684806127528805</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
         <v>5.441475566897596</v>
+      </c>
+      <c r="C25">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1731,7 +1837,7 @@
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">

</xml_diff>